<commit_message>
Updates to the manuscript
</commit_message>
<xml_diff>
--- a/Results/aggregated_efficiencies.xlsx
+++ b/Results/aggregated_efficiencies.xlsx
@@ -13,16 +13,17 @@
   </bookViews>
   <sheets>
     <sheet name="aggregated_efficiencies" sheetId="1" r:id="rId1"/>
+    <sheet name="Summary" sheetId="2" r:id="rId2"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId2"/>
+    <externalReference r:id="rId3"/>
   </externalReferences>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="71">
   <si>
     <t>Variable name</t>
   </si>
@@ -217,6 +218,24 @@
   </si>
   <si>
     <t>HotWell</t>
+  </si>
+  <si>
+    <t>SWC</t>
+  </si>
+  <si>
+    <t>LTHT merge</t>
+  </si>
+  <si>
+    <t>TC</t>
+  </si>
+  <si>
+    <t>Total TC</t>
+  </si>
+  <si>
+    <t>HVAC preheater</t>
+  </si>
+  <si>
+    <t>Steam heater</t>
   </si>
 </sst>
 </file>
@@ -713,16 +732,16 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2643,8 +2662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="J138" sqref="J138:J139"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2696,13 +2715,13 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
       <c r="F3" s="4">
         <f>[1]aggregated_efficiencies!$E$3</f>
         <v>8.6974092722049298E-2</v>
@@ -3107,8 +3126,15 @@
         <f t="shared" si="1"/>
         <v>8.0978060575160483E-3</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J16" s="6">
+        <f>I16+I5+I4</f>
+        <v>3.0186668112456544E-2</v>
+      </c>
+      <c r="K16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -3120,14 +3146,14 @@
       <c r="G17" s="2"/>
       <c r="I17" s="6"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" s="7" t="s">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A18" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
       <c r="F18" s="4">
         <f>[1]aggregated_efficiencies!$E$18</f>
         <v>0.10589052521806</v>
@@ -3135,7 +3161,7 @@
       <c r="G18" s="2"/>
       <c r="I18" s="6"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>6</v>
       </c>
@@ -3165,7 +3191,7 @@
         <v>1.0281970709353118E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
@@ -3195,7 +3221,7 @@
         <v>1.3948844172189964E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>8</v>
       </c>
@@ -3227,7 +3253,7 @@
         <v>2.5981957771534769E-20</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>9</v>
       </c>
@@ -3257,7 +3283,7 @@
         <v>1.1605976850490918E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>10</v>
       </c>
@@ -3287,7 +3313,7 @@
         <v>1.584498678884838E-4</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>11</v>
       </c>
@@ -3317,7 +3343,7 @@
         <v>7.9755339377828006E-4</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>12</v>
       </c>
@@ -3347,7 +3373,7 @@
         <v>1.9992157655444528E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>13</v>
       </c>
@@ -3377,7 +3403,7 @@
         <v>6.2279613081365629E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>14</v>
       </c>
@@ -3407,7 +3433,7 @@
         <v>9.793158553039737E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>15</v>
       </c>
@@ -3434,7 +3460,7 @@
       <c r="G28" s="2"/>
       <c r="I28" s="6"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>16</v>
       </c>
@@ -3466,7 +3492,7 @@
         <v>-4.9472426946830498E-19</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>17</v>
       </c>
@@ -3496,7 +3522,7 @@
         <v>1.7750775448129208E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>18</v>
       </c>
@@ -3525,8 +3551,15 @@
         <f t="shared" si="1"/>
         <v>9.1589234210175379E-3</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J31" s="6">
+        <f>I31+I20+I19</f>
+        <v>3.3389738302560618E-2</v>
+      </c>
+      <c r="K31" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>20</v>
       </c>
@@ -3556,7 +3589,7 @@
         <v>1.6029354788494998E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -3568,14 +3601,14 @@
       <c r="G33" s="2"/>
       <c r="I33" s="6"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A34" s="7" t="s">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A34" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
       <c r="F34" s="4">
         <f>[1]aggregated_efficiencies!$E$34</f>
         <v>0.10952400371934801</v>
@@ -3583,7 +3616,7 @@
       <c r="G34" s="2"/>
       <c r="I34" s="6"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>6</v>
       </c>
@@ -3613,7 +3646,7 @@
         <v>1.0364045619250804E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>7</v>
       </c>
@@ -3643,7 +3676,7 @@
         <v>1.3449656097520028E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>8</v>
       </c>
@@ -3675,7 +3708,7 @@
         <v>-2.9282422599315852E-20</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>9</v>
       </c>
@@ -3705,7 +3738,7 @@
         <v>1.0043574338005616E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>10</v>
       </c>
@@ -3735,7 +3768,7 @@
         <v>3.9100316105873541E-5</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>11</v>
       </c>
@@ -3765,7 +3798,7 @@
         <v>9.671021920938293E-4</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>12</v>
       </c>
@@ -3795,7 +3828,7 @@
         <v>2.0061898078007206E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>13</v>
       </c>
@@ -3825,7 +3858,7 @@
         <v>7.0075908398170381E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>14</v>
       </c>
@@ -3855,7 +3888,7 @@
         <v>1.1548127186994226E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>15</v>
       </c>
@@ -3882,7 +3915,7 @@
       <c r="G44" s="2"/>
       <c r="I44" s="6"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
         <v>16</v>
       </c>
@@ -3914,7 +3947,7 @@
         <v>-1.188500212077966E-4</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>17</v>
       </c>
@@ -3944,7 +3977,7 @@
         <v>1.9003438555349691E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
         <v>18</v>
       </c>
@@ -3973,8 +4006,15 @@
         <f t="shared" si="1"/>
         <v>9.1161464526527524E-3</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J47" s="6">
+        <f>I47+I36+I35</f>
+        <v>3.2929848169423584E-2</v>
+      </c>
+      <c r="K47" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>20</v>
       </c>
@@ -4004,7 +4044,7 @@
         <v>1.3734712934818483E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -4016,14 +4056,14 @@
       <c r="G49" s="2"/>
       <c r="I49" s="6"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A50" s="7" t="s">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A50" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B50" s="7"/>
-      <c r="C50" s="7"/>
-      <c r="D50" s="7"/>
-      <c r="E50" s="7"/>
+      <c r="B50" s="9"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
       <c r="F50" s="4">
         <f>[1]aggregated_efficiencies!$E$50</f>
         <v>9.1682502310528005E-2</v>
@@ -4031,7 +4071,7 @@
       <c r="G50" s="2"/>
       <c r="I50" s="6"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
         <v>6</v>
       </c>
@@ -4061,7 +4101,7 @@
         <v>9.5761192407525491E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
         <v>7</v>
       </c>
@@ -4091,7 +4131,7 @@
         <v>1.3385925920003535E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
         <v>8</v>
       </c>
@@ -4123,7 +4163,7 @@
         <v>-7.4619749771592349E-20</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
         <v>9</v>
       </c>
@@ -4153,7 +4193,7 @@
         <v>8.1111385966015272E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
         <v>10</v>
       </c>
@@ -4183,7 +4223,7 @@
         <v>-2.6663447543545362E-4</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
         <v>11</v>
       </c>
@@ -4213,7 +4253,7 @@
         <v>1.0658640976200329E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
         <v>12</v>
       </c>
@@ -4243,7 +4283,7 @@
         <v>2.0496548045295109E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="s">
         <v>13</v>
       </c>
@@ -4273,7 +4313,7 @@
         <v>5.459562986951598E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A59" s="2" t="s">
         <v>14</v>
       </c>
@@ -4303,7 +4343,7 @@
         <v>9.0742630213409628E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="s">
         <v>15</v>
       </c>
@@ -4330,7 +4370,7 @@
       <c r="G60" s="2"/>
       <c r="I60" s="6"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
         <v>16</v>
       </c>
@@ -4362,7 +4402,7 @@
         <v>-5.3985756005788595E-4</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
         <v>17</v>
       </c>
@@ -4392,7 +4432,7 @@
         <v>1.6861698565953311E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A63" s="2" t="s">
         <v>18</v>
       </c>
@@ -4421,8 +4461,15 @@
         <f t="shared" si="1"/>
         <v>8.0841023291583769E-3</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J63" s="6">
+        <f>I63+I52+I51</f>
+        <v>3.1046147489914459E-2</v>
+      </c>
+      <c r="K63" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -4437,14 +4484,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A65" s="7" t="s">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A65" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B65" s="7"/>
-      <c r="C65" s="7"/>
-      <c r="D65" s="7"/>
-      <c r="E65" s="7"/>
+      <c r="B65" s="9"/>
+      <c r="C65" s="9"/>
+      <c r="D65" s="9"/>
+      <c r="E65" s="9"/>
       <c r="F65" s="4">
         <f>[1]aggregated_efficiencies!$E$65</f>
         <v>0.13598580525394899</v>
@@ -4452,7 +4499,7 @@
       <c r="G65" s="2"/>
       <c r="I65" s="6"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
         <v>6</v>
       </c>
@@ -4482,7 +4529,7 @@
         <v>1.0603601192523201E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>7</v>
       </c>
@@ -4512,7 +4559,7 @@
         <v>6.1753115680829385E-3</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A68" s="2" t="s">
         <v>8</v>
       </c>
@@ -4544,7 +4591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A69" s="2" t="s">
         <v>9</v>
       </c>
@@ -4574,7 +4621,7 @@
         <v>-7.9230482458679744E-19</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A70" s="2" t="s">
         <v>10</v>
       </c>
@@ -4604,7 +4651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A71" s="2" t="s">
         <v>11</v>
       </c>
@@ -4634,7 +4681,7 @@
         <v>1.2643551380222632E-4</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="s">
         <v>12</v>
       </c>
@@ -4664,7 +4711,7 @@
         <v>1.1543916344144056E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A73" s="2" t="s">
         <v>13</v>
       </c>
@@ -4694,7 +4741,7 @@
         <v>6.4010573258668846E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A74" s="2" t="s">
         <v>14</v>
       </c>
@@ -4724,7 +4771,7 @@
         <v>1.3431534955790149E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A75" s="2" t="s">
         <v>15</v>
       </c>
@@ -4751,7 +4798,7 @@
       <c r="G75" s="2"/>
       <c r="I75" s="6"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A76" s="2" t="s">
         <v>16</v>
       </c>
@@ -4783,7 +4830,7 @@
         <v>-6.3857200293633955E-4</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A77" s="2" t="s">
         <v>17</v>
       </c>
@@ -4813,7 +4860,7 @@
         <v>2.5778186843640584E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A78" s="2" t="s">
         <v>18</v>
       </c>
@@ -4842,8 +4889,15 @@
         <f t="shared" si="6"/>
         <v>3.2078934768551226E-2</v>
       </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J78" s="6">
+        <f>I78+I67+I66</f>
+        <v>4.8857847529157367E-2</v>
+      </c>
+      <c r="K78" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A79" s="2" t="s">
         <v>20</v>
       </c>
@@ -4873,7 +4927,7 @@
         <v>2.250398663841037E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A80" s="2" t="s">
         <v>24</v>
       </c>
@@ -4903,7 +4957,7 @@
         <v>1.8107352440943743E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -4915,14 +4969,14 @@
       <c r="G81" s="2"/>
       <c r="I81" s="6"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A82" s="7" t="s">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A82" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B82" s="7"/>
-      <c r="C82" s="7"/>
-      <c r="D82" s="7"/>
-      <c r="E82" s="7"/>
+      <c r="B82" s="9"/>
+      <c r="C82" s="9"/>
+      <c r="D82" s="9"/>
+      <c r="E82" s="9"/>
       <c r="F82" s="4">
         <f>[1]aggregated_efficiencies!$E$82</f>
         <v>0.114060650314236</v>
@@ -4930,7 +4984,7 @@
       <c r="G82" s="2"/>
       <c r="I82" s="6"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A83" s="2" t="s">
         <v>6</v>
       </c>
@@ -4960,7 +5014,7 @@
         <v>9.9675191632873344E-3</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A84" s="2" t="s">
         <v>7</v>
       </c>
@@ -4990,7 +5044,7 @@
         <v>1.5375596541590259E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A85" s="2" t="s">
         <v>8</v>
       </c>
@@ -5022,7 +5076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A86" s="2" t="s">
         <v>9</v>
       </c>
@@ -5052,7 +5106,7 @@
         <v>-5.1637076134607299E-19</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A87" s="2" t="s">
         <v>10</v>
       </c>
@@ -5082,7 +5136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A88" s="2" t="s">
         <v>11</v>
       </c>
@@ -5112,7 +5166,7 @@
         <v>1.881162249172194E-4</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A89" s="2" t="s">
         <v>12</v>
       </c>
@@ -5142,7 +5196,7 @@
         <v>1.365243899626297E-3</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A90" s="2" t="s">
         <v>13</v>
       </c>
@@ -5172,7 +5226,7 @@
         <v>4.1964004553480755E-3</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A91" s="2" t="s">
         <v>14</v>
       </c>
@@ -5202,7 +5256,7 @@
         <v>9.687141014327473E-3</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A92" s="2" t="s">
         <v>15</v>
       </c>
@@ -5229,7 +5283,7 @@
       <c r="G92" s="2"/>
       <c r="I92" s="6"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A93" s="2" t="s">
         <v>16</v>
       </c>
@@ -5261,7 +5315,7 @@
         <v>-7.6967589755307033E-4</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A94" s="2" t="s">
         <v>17</v>
       </c>
@@ -5291,7 +5345,7 @@
         <v>1.6814938723343331E-3</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A95" s="2" t="s">
         <v>18</v>
       </c>
@@ -5320,8 +5374,15 @@
         <f t="shared" si="6"/>
         <v>1.2667577241009691E-2</v>
       </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J95" s="6">
+        <f>I95+I84+I83</f>
+        <v>3.8010692945887284E-2</v>
+      </c>
+      <c r="K95" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A96" s="2" t="s">
         <v>20</v>
       </c>
@@ -5351,7 +5412,7 @@
         <v>1.9826901093541932E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A97" s="2" t="s">
         <v>24</v>
       </c>
@@ -5381,7 +5442,7 @@
         <v>1.5310083344413229E-2</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -5393,14 +5454,14 @@
       <c r="G98" s="2"/>
       <c r="I98" s="6"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A99" s="7" t="s">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A99" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B99" s="7"/>
-      <c r="C99" s="7"/>
-      <c r="D99" s="7"/>
-      <c r="E99" s="7"/>
+      <c r="B99" s="9"/>
+      <c r="C99" s="9"/>
+      <c r="D99" s="9"/>
+      <c r="E99" s="9"/>
       <c r="F99" s="4">
         <f>[1]aggregated_efficiencies!$E$99</f>
         <v>0.120634669433251</v>
@@ -5408,7 +5469,7 @@
       <c r="G99" s="2"/>
       <c r="I99" s="6"/>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A100" s="2" t="s">
         <v>6</v>
       </c>
@@ -5438,7 +5499,7 @@
         <v>1.0555676412146112E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>7</v>
       </c>
@@ -5468,7 +5529,7 @@
         <v>8.5255586677693389E-3</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A102" s="2" t="s">
         <v>8</v>
       </c>
@@ -5500,7 +5561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A103" s="2" t="s">
         <v>9</v>
       </c>
@@ -5530,7 +5591,7 @@
         <v>6.7243085463010865E-19</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A104" s="2" t="s">
         <v>10</v>
       </c>
@@ -5560,7 +5621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A105" s="2" t="s">
         <v>11</v>
       </c>
@@ -5590,7 +5651,7 @@
         <v>2.125056449970841E-4</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A106" s="2" t="s">
         <v>12</v>
       </c>
@@ -5620,7 +5681,7 @@
         <v>1.5516847386702719E-3</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A107" s="2" t="s">
         <v>13</v>
       </c>
@@ -5650,7 +5711,7 @@
         <v>5.6100942611503708E-3</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A108" s="2" t="s">
         <v>14</v>
       </c>
@@ -5680,7 +5741,7 @@
         <v>1.2171276747752745E-2</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A109" s="2" t="s">
         <v>15</v>
       </c>
@@ -5707,7 +5768,7 @@
       <c r="G109" s="2"/>
       <c r="I109" s="6"/>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A110" s="2" t="s">
         <v>16</v>
       </c>
@@ -5739,7 +5800,7 @@
         <v>-2.2383251220885178E-4</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A111" s="2" t="s">
         <v>17</v>
       </c>
@@ -5769,7 +5830,7 @@
         <v>2.235458572230821E-3</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A112" s="2" t="s">
         <v>18</v>
       </c>
@@ -5797,6 +5858,13 @@
       <c r="I112" s="6">
         <f t="shared" si="6"/>
         <v>2.5492197914459631E-2</v>
+      </c>
+      <c r="J112" s="6">
+        <f>I112+I101+I100</f>
+        <v>4.4573432994375078E-2</v>
+      </c>
+      <c r="K112" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.35">
@@ -5872,13 +5940,13 @@
       <c r="I115" s="6"/>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A116" s="7" t="s">
+      <c r="A116" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B116" s="7"/>
-      <c r="C116" s="7"/>
-      <c r="D116" s="7"/>
-      <c r="E116" s="7"/>
+      <c r="B116" s="9"/>
+      <c r="C116" s="9"/>
+      <c r="D116" s="9"/>
+      <c r="E116" s="9"/>
       <c r="F116" s="4">
         <f>[1]aggregated_efficiencies!$E$116</f>
         <v>9.7017821920425296E-2</v>
@@ -6247,7 +6315,7 @@
         <v>1.8254363914459782E-3</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A129" s="2" t="s">
         <v>18</v>
       </c>
@@ -6276,8 +6344,15 @@
         <f t="shared" si="6"/>
         <v>1.9063292911064126E-2</v>
       </c>
-    </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J129" s="6">
+        <f>I129+I118+I117</f>
+        <v>3.006907423475642E-2</v>
+      </c>
+      <c r="K129" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A130" s="2" t="s">
         <v>20</v>
       </c>
@@ -6307,7 +6382,7 @@
         <v>1.4521657967379023E-2</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A131" s="2" t="s">
         <v>24</v>
       </c>
@@ -6337,7 +6412,7 @@
         <v>1.3070778200946353E-2</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A132" s="2"/>
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
@@ -6347,19 +6422,16 @@
         <v>1.0000000000000007</v>
       </c>
       <c r="G132" s="2"/>
-      <c r="I132" s="6">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A133" s="7" t="s">
+      <c r="I132" s="6"/>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A133" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B133" s="7"/>
-      <c r="C133" s="7"/>
-      <c r="D133" s="7"/>
-      <c r="E133" s="7"/>
+      <c r="B133" s="9"/>
+      <c r="C133" s="9"/>
+      <c r="D133" s="9"/>
+      <c r="E133" s="9"/>
       <c r="F133" s="4">
         <f>[1]aggregated_efficiencies!$E$133</f>
         <v>1.57433004180507E-2</v>
@@ -6367,7 +6439,7 @@
       <c r="G133" s="2"/>
       <c r="I133" s="6"/>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A134" s="2" t="s">
         <v>29</v>
       </c>
@@ -6396,12 +6468,12 @@
         <f t="shared" ref="I134:I166" si="10">F134/$I$2</f>
         <v>4.5353013308124565E-2</v>
       </c>
-      <c r="J134" s="10">
+      <c r="J134" s="7">
         <f>SUM(I134:I135)</f>
         <v>8.5169611840308065E-2</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A135" s="2" t="s">
         <v>30</v>
       </c>
@@ -6430,9 +6502,9 @@
         <f t="shared" si="10"/>
         <v>3.98165985321835E-2</v>
       </c>
-      <c r="J135" s="9"/>
-    </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J135" s="8"/>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A136" s="2" t="s">
         <v>31</v>
       </c>
@@ -6461,12 +6533,12 @@
         <f t="shared" si="10"/>
         <v>6.5299602503090211E-5</v>
       </c>
-      <c r="J136" s="10">
+      <c r="J136" s="7">
         <f>SUM(I136:I137)</f>
         <v>1.5037076230704733E-4</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A137" s="2" t="s">
         <v>32</v>
       </c>
@@ -6495,9 +6567,9 @@
         <f t="shared" si="10"/>
         <v>8.5071159803957108E-5</v>
       </c>
-      <c r="J137" s="9"/>
-    </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J137" s="8"/>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A138" s="2" t="s">
         <v>33</v>
       </c>
@@ -6526,12 +6598,12 @@
         <f t="shared" si="10"/>
         <v>-1.8277559593016354E-2</v>
       </c>
-      <c r="J138" s="10">
+      <c r="J138" s="7">
         <f>SUM(I138:I139)</f>
         <v>-3.3264746450482816E-2</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A139" s="2" t="s">
         <v>34</v>
       </c>
@@ -6560,9 +6632,9 @@
         <f t="shared" si="10"/>
         <v>-1.498718685746646E-2</v>
       </c>
-      <c r="J139" s="9"/>
-    </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J139" s="8"/>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A140" s="3" t="s">
         <v>35</v>
       </c>
@@ -6593,12 +6665,12 @@
         <f t="shared" si="10"/>
         <v>-8.4767697504216247E-4</v>
       </c>
-      <c r="J140" s="10">
+      <c r="J140" s="7">
         <f>SUM(I140:I141)</f>
         <v>-1.6937947724295437E-3</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A141" s="3" t="s">
         <v>36</v>
       </c>
@@ -6629,9 +6701,9 @@
         <f t="shared" si="10"/>
         <v>-8.4611779738738135E-4</v>
       </c>
-      <c r="J141" s="9"/>
-    </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J141" s="8"/>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A142" s="2" t="s">
         <v>37</v>
       </c>
@@ -6660,12 +6732,12 @@
         <f t="shared" si="10"/>
         <v>8.6828773213740718E-3</v>
       </c>
-      <c r="J142" s="10">
+      <c r="J142" s="7">
         <f>SUM(I142:I143)</f>
         <v>1.6044159167855041E-2</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A143" s="2" t="s">
         <v>38</v>
       </c>
@@ -6694,9 +6766,9 @@
         <f t="shared" si="10"/>
         <v>7.3612818464809703E-3</v>
       </c>
-      <c r="J143" s="9"/>
-    </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J143" s="8"/>
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A144" s="2" t="s">
         <v>39</v>
       </c>
@@ -6727,7 +6799,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="J144" s="10">
+      <c r="J144" s="7">
         <f>SUM(I144:I145)</f>
         <v>0</v>
       </c>
@@ -6763,7 +6835,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="J145" s="9"/>
+      <c r="J145" s="8"/>
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.35">
       <c r="E146" s="2">
@@ -6776,13 +6848,13 @@
       </c>
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A147" s="8" t="s">
+      <c r="A147" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B147" s="8"/>
-      <c r="C147" s="8"/>
-      <c r="D147" s="8"/>
-      <c r="E147" s="8"/>
+      <c r="B147" s="10"/>
+      <c r="C147" s="10"/>
+      <c r="D147" s="10"/>
+      <c r="E147" s="10"/>
       <c r="F147" s="4">
         <f>[1]aggregated_efficiencies!$E$147</f>
         <v>5.3744207319153199E-2</v>
@@ -6817,7 +6889,7 @@
         <f t="shared" si="10"/>
         <v>3.537427692613481E-3</v>
       </c>
-      <c r="J148" s="10">
+      <c r="J148" s="7">
         <f>SUM(I148:I149)</f>
         <v>8.7403223501491892E-3</v>
       </c>
@@ -6850,7 +6922,7 @@
         <f t="shared" si="10"/>
         <v>5.2028946575357077E-3</v>
       </c>
-      <c r="J149" s="9"/>
+      <c r="J149" s="8"/>
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A150" s="2" t="s">
@@ -7047,13 +7119,13 @@
       </c>
     </row>
     <row r="157" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A157" s="7" t="s">
+      <c r="A157" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B157" s="7"/>
-      <c r="C157" s="7"/>
-      <c r="D157" s="7"/>
-      <c r="E157" s="7"/>
+      <c r="B157" s="9"/>
+      <c r="C157" s="9"/>
+      <c r="D157" s="9"/>
+      <c r="E157" s="9"/>
       <c r="F157" s="4">
         <f>[1]aggregated_efficiencies!$E$157</f>
         <v>6.8742421370945897E-2</v>
@@ -7333,6 +7405,17 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A99:E99"/>
+    <mergeCell ref="A116:E116"/>
+    <mergeCell ref="A133:E133"/>
+    <mergeCell ref="A147:E147"/>
+    <mergeCell ref="A157:E157"/>
+    <mergeCell ref="A82:E82"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="A34:E34"/>
+    <mergeCell ref="A50:E50"/>
+    <mergeCell ref="A65:E65"/>
     <mergeCell ref="J144:J145"/>
     <mergeCell ref="J148:J149"/>
     <mergeCell ref="J134:J135"/>
@@ -7340,17 +7423,6 @@
     <mergeCell ref="J138:J139"/>
     <mergeCell ref="J140:J141"/>
     <mergeCell ref="J142:J143"/>
-    <mergeCell ref="A82:E82"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A18:E18"/>
-    <mergeCell ref="A34:E34"/>
-    <mergeCell ref="A50:E50"/>
-    <mergeCell ref="A65:E65"/>
-    <mergeCell ref="A99:E99"/>
-    <mergeCell ref="A116:E116"/>
-    <mergeCell ref="A133:E133"/>
-    <mergeCell ref="A147:E147"/>
-    <mergeCell ref="A157:E157"/>
   </mergeCells>
   <conditionalFormatting sqref="F1:F1048576">
     <cfRule type="colorScale" priority="3">
@@ -7379,4 +7451,94 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="6">
+        <f>aggregated_efficiencies!J148</f>
+        <v>8.7403223501491892E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="6">
+        <f>aggregated_efficiencies!J134</f>
+        <v>8.5169611840308065E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="6">
+        <f>aggregated_efficiencies!I32+aggregated_efficiencies!I48+aggregated_efficiencies!I79+aggregated_efficiencies!I96+aggregated_efficiencies!I113+aggregated_efficiencies!I130</f>
+        <v>0.10726000673222025</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="6">
+        <f>aggregated_efficiencies!J142</f>
+        <v>1.6044159167855041E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="6">
+        <f>aggregated_efficiencies!J16+aggregated_efficiencies!J31+aggregated_efficiencies!J47+aggregated_efficiencies!J63+aggregated_efficiencies!J78+aggregated_efficiencies!J95+aggregated_efficiencies!J112+aggregated_efficiencies!J129</f>
+        <v>0.28906344977853132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="6">
+        <f>aggregated_efficiencies!I80+aggregated_efficiencies!I97+aggregated_efficiencies!I114+aggregated_efficiencies!I131</f>
+        <v>6.0543083624771267E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="6">
+        <f>aggregated_efficiencies!I152</f>
+        <v>0.10352810823738808</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="6">
+        <f>aggregated_efficiencies!I154</f>
+        <v>0.10493464081965476</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>